<commit_message>
Actualización de Redes (Constanza Pérez)
</commit_message>
<xml_diff>
--- a/Datos/coes_2015.xlsx
+++ b/Datos/coes_2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmunozrojas/pCloud Sync/7_COES/5_Otros/Redes_COES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmunozrojas/pCloud Sync/7_COES/5_Otros/Redes_COES/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA44999E-509D-B94E-B7AA-92B75E1B0A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09F0EDCA-C495-FE49-B576-328954DAD2A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="14940" xr2:uid="{37AD07C9-C76A-384D-B0E9-1FDE6BAFED24}"/>
+    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="14940" xr2:uid="{3E4083E2-A3E1-4740-A18E-BE3A5664177B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,143 +32,143 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
-    <t>Alfredo Joignant</t>
+    <t>A. Joignant</t>
   </si>
   <si>
-    <t>Ana Figueiredo</t>
+    <t>A. Figueiredo</t>
   </si>
   <si>
-    <t>Ana Velitchkova</t>
+    <t>A. Velitchkova</t>
   </si>
   <si>
-    <t>Claudia Heiss</t>
+    <t>C. Heiss</t>
   </si>
   <si>
-    <t>Claudia Sanhueza</t>
+    <t>C. Sanhueza</t>
   </si>
   <si>
-    <t>Claudio Rolle</t>
+    <t>C. Rolle</t>
   </si>
   <si>
-    <t>Cristian Doñas</t>
+    <t>C. Doñas</t>
   </si>
   <si>
-    <t>Daniel Hojman</t>
+    <t>D. Hojman</t>
   </si>
   <si>
-    <t>Dante Contreras</t>
+    <t>D. Contreras</t>
   </si>
   <si>
-    <t>Dariela Sharim</t>
+    <t>D. Sharim</t>
   </si>
   <si>
-    <t>Emmanuelle Barozet</t>
+    <t>E. Barozet</t>
   </si>
   <si>
-    <t>Ernesto López</t>
+    <t>E. López</t>
   </si>
   <si>
-    <t>Fabian Duarte</t>
+    <t>F. Duarte</t>
   </si>
   <si>
-    <t>Felipe Link</t>
+    <t>F. Link</t>
   </si>
   <si>
-    <t>Francisca Gutiérrez</t>
+    <t>F. Gutiérrez</t>
   </si>
   <si>
-    <t>Gloria Jiménez-Moya</t>
+    <t>G. Jiménez-Moya</t>
   </si>
   <si>
-    <t>Héctor Carvacho</t>
+    <t>H. Carvacho</t>
   </si>
   <si>
-    <t>Hugo Romero</t>
+    <t>H. Romero</t>
   </si>
   <si>
-    <t>Ismael Puga</t>
+    <t>I. Puga</t>
   </si>
   <si>
-    <t>Javier Couso</t>
+    <t>J. Couso</t>
   </si>
   <si>
-    <t>Jorge Atria</t>
+    <t>J. Atria</t>
   </si>
   <si>
-    <t>Juan Carlos Castillo</t>
+    <t>JC. Castillo</t>
   </si>
   <si>
-    <t>Kirsten Sehnbruch</t>
+    <t>K. Sehnbruch</t>
   </si>
   <si>
-    <t>Luis Valenzuela</t>
+    <t>L. Valenzuela</t>
   </si>
   <si>
-    <t>María Luisa Méndez</t>
+    <t>ML. Méndez</t>
   </si>
   <si>
-    <t>Matías Bargsted</t>
+    <t>M. Bargsted</t>
   </si>
   <si>
-    <t>Matías Garretón</t>
+    <t>M. Garretón</t>
   </si>
   <si>
-    <t>Matías Sanfuentes</t>
+    <t>M. Sanfuentes</t>
   </si>
   <si>
-    <t>Mauricio Morales</t>
+    <t>M. Morales</t>
   </si>
   <si>
-    <t>Mauro Basaure</t>
+    <t>M. Basaure</t>
   </si>
   <si>
-    <t>Mónica Gerber</t>
+    <t>M. Gerber</t>
   </si>
   <si>
-    <t>Nicolás Angelcos</t>
+    <t>N. Angelcos</t>
   </si>
   <si>
-    <t>Nicolás Grau</t>
+    <t>N. Grau</t>
   </si>
   <si>
-    <t>Nicolás Somma</t>
+    <t>N. Somma</t>
   </si>
   <si>
-    <t>Pablo De Tezanos</t>
+    <t>P. De Tezanos</t>
   </si>
   <si>
-    <t>Pablo Gonzalez</t>
+    <t>P. González</t>
   </si>
   <si>
-    <t>Paola Bordón</t>
+    <t>P. Bordón</t>
   </si>
   <si>
-    <t>Patricio Aroca</t>
+    <t>P. Aroca</t>
   </si>
   <si>
-    <t>Patricio Cumsille</t>
+    <t>P. Cumsille</t>
   </si>
   <si>
-    <t>Patricio Navia</t>
+    <t>P. Navia</t>
   </si>
   <si>
-    <t>Paula Luengo</t>
+    <t>P. Luengo</t>
   </si>
   <si>
-    <t>Roberto González</t>
+    <t>R. González</t>
   </si>
   <si>
-    <t>Sofía Donoso</t>
+    <t>S. Donoso</t>
   </si>
   <si>
-    <t>Vicente Espinoza</t>
+    <t>V. Espinoza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,13 +184,23 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,7 +215,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE045AB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,6 +247,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -236,13 +282,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -558,7 +631,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92A9B90-4E41-284C-9EE9-16E3FC4635B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2C1CF8-66BA-5040-A37F-9A7A0BC6854C}">
   <dimension ref="A1:AS45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -706,7 +779,7 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -769,7 +842,7 @@
       <c r="V2" s="1">
         <v>0</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="4">
         <v>1</v>
       </c>
       <c r="X2" s="1">
@@ -790,11 +863,11 @@
       <c r="AC2" s="1">
         <v>0</v>
       </c>
-      <c r="AD2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>0</v>
+      <c r="AD2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>1</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
@@ -846,10 +919,10 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
         <v>1</v>
       </c>
       <c r="E3" s="1">
@@ -885,10 +958,10 @@
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="3">
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
         <v>1</v>
       </c>
       <c r="R3" s="1">
@@ -963,13 +1036,13 @@
       <c r="AO3" s="1">
         <v>0</v>
       </c>
-      <c r="AP3" s="3">
+      <c r="AP3" s="6">
         <v>1</v>
       </c>
       <c r="AQ3" s="1">
         <v>0</v>
       </c>
-      <c r="AR3" s="3">
+      <c r="AR3" s="6">
         <v>1</v>
       </c>
       <c r="AS3" s="1">
@@ -983,10 +1056,10 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>0</v>
       </c>
       <c r="E4" s="1">
@@ -1022,10 +1095,10 @@
       <c r="O4" s="1">
         <v>0</v>
       </c>
-      <c r="P4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="3">
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6">
         <v>1</v>
       </c>
       <c r="R4" s="1">
@@ -1100,13 +1173,13 @@
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AP4" s="6">
         <v>1</v>
       </c>
       <c r="AQ4" s="1">
         <v>0</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AR4" s="6">
         <v>1</v>
       </c>
       <c r="AS4" s="1">
@@ -1126,7 +1199,7 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="1">
@@ -1266,7 +1339,7 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
       <c r="G6" s="1">
@@ -1284,10 +1357,10 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
         <v>1</v>
       </c>
       <c r="N6" s="1">
@@ -1406,7 +1479,7 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7" s="1">
@@ -1546,7 +1619,7 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>0</v>
       </c>
       <c r="I8" s="1">
@@ -1686,7 +1759,7 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="1">
@@ -1695,13 +1768,13 @@
       <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="L9" s="1">
-        <v>0</v>
+      <c r="L9" s="8">
+        <v>1</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="9">
         <v>1</v>
       </c>
       <c r="O9" s="1">
@@ -1728,14 +1801,14 @@
       <c r="V9" s="1">
         <v>0</v>
       </c>
-      <c r="W9" s="1">
-        <v>0</v>
+      <c r="W9" s="10">
+        <v>1</v>
       </c>
       <c r="X9" s="1">
         <v>0</v>
       </c>
-      <c r="Y9" s="1">
-        <v>0</v>
+      <c r="Y9" s="4">
+        <v>1</v>
       </c>
       <c r="Z9" s="1">
         <v>0</v>
@@ -1761,7 +1834,7 @@
       <c r="AG9" s="1">
         <v>0</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AH9" s="10">
         <v>1</v>
       </c>
       <c r="AI9" s="1">
@@ -1776,7 +1849,7 @@
       <c r="AL9" s="1">
         <v>0</v>
       </c>
-      <c r="AM9" s="3">
+      <c r="AM9" s="10">
         <v>1</v>
       </c>
       <c r="AN9" s="1">
@@ -1791,7 +1864,7 @@
       <c r="AQ9" s="1">
         <v>0</v>
       </c>
-      <c r="AR9" s="3">
+      <c r="AR9" s="10">
         <v>1</v>
       </c>
       <c r="AS9" s="1">
@@ -1826,7 +1899,7 @@
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" s="1">
@@ -1841,8 +1914,8 @@
       <c r="N10" s="1">
         <v>0</v>
       </c>
-      <c r="O10" s="1">
-        <v>0</v>
+      <c r="O10" s="6">
+        <v>1</v>
       </c>
       <c r="P10" s="1">
         <v>0</v>
@@ -1874,8 +1947,8 @@
       <c r="Y10" s="1">
         <v>0</v>
       </c>
-      <c r="Z10" s="1">
-        <v>0</v>
+      <c r="Z10" s="6">
+        <v>1</v>
       </c>
       <c r="AA10" s="1">
         <v>0</v>
@@ -1904,8 +1977,8 @@
       <c r="AI10" s="1">
         <v>0</v>
       </c>
-      <c r="AJ10" s="1">
-        <v>0</v>
+      <c r="AJ10" s="6">
+        <v>1</v>
       </c>
       <c r="AK10" s="1">
         <v>0</v>
@@ -1922,7 +1995,7 @@
       <c r="AO10" s="1">
         <v>0</v>
       </c>
-      <c r="AP10" s="3">
+      <c r="AP10" s="11">
         <v>1</v>
       </c>
       <c r="AQ10" s="1">
@@ -1966,7 +2039,7 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="3">
         <v>0</v>
       </c>
       <c r="L11" s="1">
@@ -2088,8 +2161,8 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <v>0</v>
+      <c r="F12" s="6">
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -2097,8 +2170,8 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1">
-        <v>0</v>
+      <c r="I12" s="8">
+        <v>1</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
@@ -2106,7 +2179,7 @@
       <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="1">
@@ -2142,7 +2215,7 @@
       <c r="W12" s="1">
         <v>0</v>
       </c>
-      <c r="X12" s="3">
+      <c r="X12" s="11">
         <v>1</v>
       </c>
       <c r="Y12" s="1">
@@ -2175,8 +2248,8 @@
       <c r="AH12" s="1">
         <v>0</v>
       </c>
-      <c r="AI12" s="1">
-        <v>0</v>
+      <c r="AI12" s="11">
+        <v>1</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
@@ -2225,7 +2298,7 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="11">
         <v>1</v>
       </c>
       <c r="G13" s="1">
@@ -2246,13 +2319,13 @@
       <c r="L13" s="1">
         <v>0</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="3">
         <v>0</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="4">
         <v>1</v>
       </c>
       <c r="P13" s="1">
@@ -2285,7 +2358,7 @@
       <c r="Y13" s="1">
         <v>0</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13" s="6">
         <v>1</v>
       </c>
       <c r="AA13" s="1">
@@ -2315,7 +2388,7 @@
       <c r="AI13" s="1">
         <v>0</v>
       </c>
-      <c r="AJ13" s="4">
+      <c r="AJ13" s="6">
         <v>1</v>
       </c>
       <c r="AK13" s="1">
@@ -2371,7 +2444,7 @@
       <c r="H14" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="9">
         <v>1</v>
       </c>
       <c r="J14" s="1">
@@ -2386,7 +2459,7 @@
       <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="3">
         <v>0</v>
       </c>
       <c r="O14" s="1">
@@ -2511,8 +2584,8 @@
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="1">
-        <v>0</v>
+      <c r="J15" s="6">
+        <v>1</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
@@ -2520,13 +2593,13 @@
       <c r="L15" s="1">
         <v>0</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="4">
         <v>1</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="3">
         <v>0</v>
       </c>
       <c r="P15" s="1">
@@ -2559,7 +2632,7 @@
       <c r="Y15" s="1">
         <v>0</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15" s="6">
         <v>1</v>
       </c>
       <c r="AA15" s="1">
@@ -2589,7 +2662,7 @@
       <c r="AI15" s="1">
         <v>0</v>
       </c>
-      <c r="AJ15" s="4">
+      <c r="AJ15" s="6">
         <v>1</v>
       </c>
       <c r="AK15" s="1">
@@ -2627,10 +2700,10 @@
       <c r="B16" s="1">
         <v>0</v>
       </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
       <c r="E16" s="1">
@@ -2666,13 +2739,13 @@
       <c r="O16" s="1">
         <v>0</v>
       </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="3">
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>1</v>
+      </c>
+      <c r="R16" s="7">
         <v>1</v>
       </c>
       <c r="S16" s="1">
@@ -2744,13 +2817,13 @@
       <c r="AO16" s="1">
         <v>0</v>
       </c>
-      <c r="AP16" s="3">
+      <c r="AP16" s="6">
         <v>1</v>
       </c>
       <c r="AQ16" s="1">
         <v>0</v>
       </c>
-      <c r="AR16" s="3">
+      <c r="AR16" s="6">
         <v>1</v>
       </c>
       <c r="AS16" s="1">
@@ -2764,10 +2837,10 @@
       <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="1">
@@ -2803,13 +2876,13 @@
       <c r="O17" s="1">
         <v>0</v>
       </c>
-      <c r="P17" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>0</v>
-      </c>
-      <c r="R17" s="3">
+      <c r="P17" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
         <v>1</v>
       </c>
       <c r="S17" s="1">
@@ -2851,8 +2924,8 @@
       <c r="AE17" s="1">
         <v>0</v>
       </c>
-      <c r="AF17" s="1">
-        <v>0</v>
+      <c r="AF17" s="11">
+        <v>1</v>
       </c>
       <c r="AG17" s="1">
         <v>0</v>
@@ -2881,13 +2954,13 @@
       <c r="AO17" s="1">
         <v>0</v>
       </c>
-      <c r="AP17" s="3">
+      <c r="AP17" s="11">
         <v>1</v>
       </c>
       <c r="AQ17" s="1">
         <v>0</v>
       </c>
-      <c r="AR17" s="3">
+      <c r="AR17" s="6">
         <v>1</v>
       </c>
       <c r="AS17" s="1">
@@ -2943,10 +3016,10 @@
       <c r="P18" s="1">
         <v>0</v>
       </c>
-      <c r="Q18" s="3">
-        <v>1</v>
-      </c>
-      <c r="R18" s="1">
+      <c r="Q18" s="6">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
         <v>0</v>
       </c>
       <c r="S18" s="1">
@@ -2988,7 +3061,7 @@
       <c r="AE18" s="1">
         <v>0</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AF18" s="11">
         <v>1</v>
       </c>
       <c r="AG18" s="1">
@@ -3021,7 +3094,7 @@
       <c r="AP18" s="1">
         <v>0</v>
       </c>
-      <c r="AQ18" s="4">
+      <c r="AQ18" s="9">
         <v>1</v>
       </c>
       <c r="AR18" s="1">
@@ -3086,7 +3159,7 @@
       <c r="R19" s="1">
         <v>0</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" s="3">
         <v>0</v>
       </c>
       <c r="T19" s="1">
@@ -3226,7 +3299,7 @@
       <c r="S20" s="1">
         <v>0</v>
       </c>
-      <c r="T20" s="1">
+      <c r="T20" s="3">
         <v>0</v>
       </c>
       <c r="U20" s="1">
@@ -3262,7 +3335,7 @@
       <c r="AE20" s="1">
         <v>0</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AF20" s="11">
         <v>1</v>
       </c>
       <c r="AG20" s="1">
@@ -3366,7 +3439,7 @@
       <c r="T21" s="1">
         <v>0</v>
       </c>
-      <c r="U21" s="1">
+      <c r="U21" s="3">
         <v>0</v>
       </c>
       <c r="V21" s="1">
@@ -3506,7 +3579,7 @@
       <c r="U22" s="1">
         <v>0</v>
       </c>
-      <c r="V22" s="1">
+      <c r="V22" s="3">
         <v>0</v>
       </c>
       <c r="W22" s="1">
@@ -3583,7 +3656,7 @@
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="1">
@@ -3604,8 +3677,8 @@
       <c r="H23" s="1">
         <v>0</v>
       </c>
-      <c r="I23" s="1">
-        <v>0</v>
+      <c r="I23" s="10">
+        <v>1</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
@@ -3646,7 +3719,7 @@
       <c r="V23" s="1">
         <v>0</v>
       </c>
-      <c r="W23" s="1">
+      <c r="W23" s="3">
         <v>0</v>
       </c>
       <c r="X23" s="1">
@@ -3658,7 +3731,7 @@
       <c r="Z23" s="1">
         <v>0</v>
       </c>
-      <c r="AA23" s="3">
+      <c r="AA23" s="7">
         <v>1</v>
       </c>
       <c r="AB23" s="1">
@@ -3697,8 +3770,8 @@
       <c r="AM23" s="1">
         <v>0</v>
       </c>
-      <c r="AN23" s="1">
-        <v>0</v>
+      <c r="AN23" s="11">
+        <v>1</v>
       </c>
       <c r="AO23" s="1">
         <v>0</v>
@@ -3732,8 +3805,8 @@
       <c r="E24" s="1">
         <v>0</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
+      <c r="F24" s="7">
+        <v>1</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -3750,7 +3823,7 @@
       <c r="K24" s="1">
         <v>0</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="11">
         <v>1</v>
       </c>
       <c r="M24" s="1">
@@ -3786,7 +3859,7 @@
       <c r="W24" s="1">
         <v>0</v>
       </c>
-      <c r="X24" s="1">
+      <c r="X24" s="3">
         <v>0</v>
       </c>
       <c r="Y24" s="1">
@@ -3825,7 +3898,7 @@
       <c r="AJ24" s="1">
         <v>0</v>
       </c>
-      <c r="AK24" s="4">
+      <c r="AK24" s="11">
         <v>1</v>
       </c>
       <c r="AL24" s="1">
@@ -3846,8 +3919,8 @@
       <c r="AQ24" s="1">
         <v>0</v>
       </c>
-      <c r="AR24" s="1">
-        <v>0</v>
+      <c r="AR24" s="11">
+        <v>1</v>
       </c>
       <c r="AS24" s="1">
         <v>0</v>
@@ -3878,8 +3951,8 @@
       <c r="H25" s="1">
         <v>0</v>
       </c>
-      <c r="I25" s="1">
-        <v>0</v>
+      <c r="I25" s="4">
+        <v>1</v>
       </c>
       <c r="J25" s="1">
         <v>0</v>
@@ -3926,26 +3999,26 @@
       <c r="X25" s="1">
         <v>0</v>
       </c>
-      <c r="Y25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="3">
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="7">
         <v>1</v>
       </c>
       <c r="AA25" s="1">
         <v>0</v>
       </c>
-      <c r="AB25" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="3">
+      <c r="AB25" s="12">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="12">
         <v>1</v>
       </c>
       <c r="AD25" s="1">
         <v>0</v>
       </c>
-      <c r="AE25" s="3">
-        <v>1</v>
+      <c r="AE25" s="13">
+        <v>0</v>
       </c>
       <c r="AF25" s="1">
         <v>0</v>
@@ -3959,8 +4032,8 @@
       <c r="AI25" s="1">
         <v>0</v>
       </c>
-      <c r="AJ25" s="1">
-        <v>0</v>
+      <c r="AJ25" s="12">
+        <v>1</v>
       </c>
       <c r="AK25" s="1">
         <v>0</v>
@@ -3980,8 +4053,8 @@
       <c r="AP25" s="1">
         <v>0</v>
       </c>
-      <c r="AQ25" s="1">
-        <v>0</v>
+      <c r="AQ25" s="11">
+        <v>1</v>
       </c>
       <c r="AR25" s="1">
         <v>0</v>
@@ -4018,8 +4091,8 @@
       <c r="I26" s="1">
         <v>0</v>
       </c>
-      <c r="J26" s="1">
-        <v>0</v>
+      <c r="J26" s="6">
+        <v>1</v>
       </c>
       <c r="K26" s="1">
         <v>0</v>
@@ -4027,13 +4100,13 @@
       <c r="L26" s="1">
         <v>0</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26" s="4">
         <v>1</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="6">
         <v>1</v>
       </c>
       <c r="P26" s="1">
@@ -4063,10 +4136,10 @@
       <c r="X26" s="1">
         <v>0</v>
       </c>
-      <c r="Y26" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="1">
+      <c r="Y26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="3">
         <v>0</v>
       </c>
       <c r="AA26" s="1">
@@ -4081,8 +4154,8 @@
       <c r="AD26" s="1">
         <v>0</v>
       </c>
-      <c r="AE26" s="3">
-        <v>1</v>
+      <c r="AE26" s="1">
+        <v>0</v>
       </c>
       <c r="AF26" s="1">
         <v>0</v>
@@ -4096,7 +4169,7 @@
       <c r="AI26" s="1">
         <v>0</v>
       </c>
-      <c r="AJ26" s="4">
+      <c r="AJ26" s="6">
         <v>1</v>
       </c>
       <c r="AK26" s="1">
@@ -4194,7 +4267,7 @@
       <c r="V27" s="1">
         <v>0</v>
       </c>
-      <c r="W27" s="3">
+      <c r="W27" s="7">
         <v>1</v>
       </c>
       <c r="X27" s="1">
@@ -4206,7 +4279,7 @@
       <c r="Z27" s="1">
         <v>0</v>
       </c>
-      <c r="AA27" s="1">
+      <c r="AA27" s="3">
         <v>0</v>
       </c>
       <c r="AB27" s="1">
@@ -4230,7 +4303,7 @@
       <c r="AH27" s="1">
         <v>0</v>
       </c>
-      <c r="AI27" s="3">
+      <c r="AI27" s="7">
         <v>1</v>
       </c>
       <c r="AJ27" s="1">
@@ -4260,8 +4333,8 @@
       <c r="AR27" s="1">
         <v>0</v>
       </c>
-      <c r="AS27" s="1">
-        <v>0</v>
+      <c r="AS27" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.2">
@@ -4337,7 +4410,7 @@
       <c r="X28" s="1">
         <v>0</v>
       </c>
-      <c r="Y28" s="3">
+      <c r="Y28" s="12">
         <v>1</v>
       </c>
       <c r="Z28" s="1">
@@ -4346,10 +4419,10 @@
       <c r="AA28" s="1">
         <v>0</v>
       </c>
-      <c r="AB28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="3">
+      <c r="AB28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="12">
         <v>1</v>
       </c>
       <c r="AD28" s="1">
@@ -4474,7 +4547,7 @@
       <c r="X29" s="1">
         <v>0</v>
       </c>
-      <c r="Y29" s="3">
+      <c r="Y29" s="12">
         <v>1</v>
       </c>
       <c r="Z29" s="1">
@@ -4483,10 +4556,10 @@
       <c r="AA29" s="1">
         <v>0</v>
       </c>
-      <c r="AB29" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC29" s="1">
+      <c r="AB29" s="12">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="3">
         <v>0</v>
       </c>
       <c r="AD29" s="1">
@@ -4542,7 +4615,7 @@
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="7">
         <v>1</v>
       </c>
       <c r="C30" s="1">
@@ -4626,7 +4699,7 @@
       <c r="AC30" s="1">
         <v>0</v>
       </c>
-      <c r="AD30" s="1">
+      <c r="AD30" s="3">
         <v>0</v>
       </c>
       <c r="AE30" s="1">
@@ -4679,8 +4752,8 @@
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
+      <c r="B31" s="4">
+        <v>1</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -4748,11 +4821,11 @@
       <c r="X31" s="1">
         <v>0</v>
       </c>
-      <c r="Y31" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z31" s="3">
-        <v>1</v>
+      <c r="Y31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>0</v>
       </c>
       <c r="AA31" s="1">
         <v>0</v>
@@ -4766,7 +4839,7 @@
       <c r="AD31" s="1">
         <v>0</v>
       </c>
-      <c r="AE31" s="1">
+      <c r="AE31" s="3">
         <v>0</v>
       </c>
       <c r="AF31" s="1">
@@ -4805,8 +4878,8 @@
       <c r="AQ31" s="1">
         <v>0</v>
       </c>
-      <c r="AR31" s="1">
-        <v>0</v>
+      <c r="AR31" s="14">
+        <v>1</v>
       </c>
       <c r="AS31" s="1">
         <v>0</v>
@@ -4861,16 +4934,16 @@
       <c r="P32" s="1">
         <v>0</v>
       </c>
-      <c r="Q32" s="3">
-        <v>1</v>
-      </c>
-      <c r="R32" s="3">
+      <c r="Q32" s="11">
+        <v>1</v>
+      </c>
+      <c r="R32" s="11">
         <v>1</v>
       </c>
       <c r="S32" s="1">
         <v>0</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32" s="11">
         <v>1</v>
       </c>
       <c r="U32" s="1">
@@ -4906,7 +4979,7 @@
       <c r="AE32" s="1">
         <v>0</v>
       </c>
-      <c r="AF32" s="1">
+      <c r="AF32" s="3">
         <v>0</v>
       </c>
       <c r="AG32" s="1">
@@ -4915,7 +4988,7 @@
       <c r="AH32" s="1">
         <v>0</v>
       </c>
-      <c r="AI32" s="3">
+      <c r="AI32" s="7">
         <v>1</v>
       </c>
       <c r="AJ32" s="1">
@@ -4939,10 +5012,10 @@
       <c r="AP32" s="1">
         <v>0</v>
       </c>
-      <c r="AQ32" s="4">
-        <v>1</v>
-      </c>
-      <c r="AR32" s="3">
+      <c r="AQ32" s="9">
+        <v>1</v>
+      </c>
+      <c r="AR32" s="7">
         <v>1</v>
       </c>
       <c r="AS32" s="1">
@@ -5046,7 +5119,7 @@
       <c r="AF33" s="1">
         <v>0</v>
       </c>
-      <c r="AG33" s="1">
+      <c r="AG33" s="3">
         <v>0</v>
       </c>
       <c r="AH33" s="1">
@@ -5111,7 +5184,7 @@
       <c r="H34" s="1">
         <v>0</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="10">
         <v>1</v>
       </c>
       <c r="J34" s="1">
@@ -5186,7 +5259,7 @@
       <c r="AG34" s="1">
         <v>0</v>
       </c>
-      <c r="AH34" s="1">
+      <c r="AH34" s="3">
         <v>0</v>
       </c>
       <c r="AI34" s="1">
@@ -5216,7 +5289,7 @@
       <c r="AQ34" s="1">
         <v>0</v>
       </c>
-      <c r="AR34" s="3">
+      <c r="AR34" s="10">
         <v>1</v>
       </c>
       <c r="AS34" s="1">
@@ -5257,8 +5330,8 @@
       <c r="K35" s="1">
         <v>0</v>
       </c>
-      <c r="L35" s="1">
-        <v>0</v>
+      <c r="L35" s="11">
+        <v>1</v>
       </c>
       <c r="M35" s="1">
         <v>0</v>
@@ -5302,7 +5375,7 @@
       <c r="Z35" s="1">
         <v>0</v>
       </c>
-      <c r="AA35" s="3">
+      <c r="AA35" s="7">
         <v>1</v>
       </c>
       <c r="AB35" s="1">
@@ -5317,7 +5390,7 @@
       <c r="AE35" s="1">
         <v>0</v>
       </c>
-      <c r="AF35" s="3">
+      <c r="AF35" s="7">
         <v>1</v>
       </c>
       <c r="AG35" s="1">
@@ -5326,7 +5399,7 @@
       <c r="AH35" s="1">
         <v>0</v>
       </c>
-      <c r="AI35" s="1">
+      <c r="AI35" s="3">
         <v>0</v>
       </c>
       <c r="AJ35" s="1">
@@ -5353,7 +5426,7 @@
       <c r="AQ35" s="1">
         <v>0</v>
       </c>
-      <c r="AR35" s="3">
+      <c r="AR35" s="7">
         <v>1</v>
       </c>
       <c r="AS35" s="1">
@@ -5388,8 +5461,8 @@
       <c r="I36" s="1">
         <v>0</v>
       </c>
-      <c r="J36" s="1">
-        <v>0</v>
+      <c r="J36" s="6">
+        <v>1</v>
       </c>
       <c r="K36" s="1">
         <v>0</v>
@@ -5397,13 +5470,13 @@
       <c r="L36" s="1">
         <v>0</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M36" s="4">
         <v>1</v>
       </c>
       <c r="N36" s="1">
         <v>0</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="6">
         <v>1</v>
       </c>
       <c r="P36" s="1">
@@ -5433,10 +5506,10 @@
       <c r="X36" s="1">
         <v>0</v>
       </c>
-      <c r="Y36" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="3">
+      <c r="Y36" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="6">
         <v>1</v>
       </c>
       <c r="AA36" s="1">
@@ -5466,7 +5539,7 @@
       <c r="AI36" s="1">
         <v>0</v>
       </c>
-      <c r="AJ36" s="1">
+      <c r="AJ36" s="3">
         <v>0</v>
       </c>
       <c r="AK36" s="1">
@@ -5487,7 +5560,7 @@
       <c r="AP36" s="1">
         <v>0</v>
       </c>
-      <c r="AQ36" s="4">
+      <c r="AQ36" s="9">
         <v>1</v>
       </c>
       <c r="AR36" s="1">
@@ -5567,7 +5640,7 @@
       <c r="W37" s="1">
         <v>0</v>
       </c>
-      <c r="X37" s="3">
+      <c r="X37" s="11">
         <v>1</v>
       </c>
       <c r="Y37" s="1">
@@ -5606,7 +5679,7 @@
       <c r="AJ37" s="1">
         <v>0</v>
       </c>
-      <c r="AK37" s="1">
+      <c r="AK37" s="3">
         <v>0</v>
       </c>
       <c r="AL37" s="1">
@@ -5746,7 +5819,7 @@
       <c r="AK38" s="1">
         <v>0</v>
       </c>
-      <c r="AL38" s="1">
+      <c r="AL38" s="3">
         <v>0</v>
       </c>
       <c r="AM38" s="1">
@@ -5796,7 +5869,7 @@
       <c r="H39" s="1">
         <v>0</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="10">
         <v>1</v>
       </c>
       <c r="J39" s="1">
@@ -5886,7 +5959,7 @@
       <c r="AL39" s="1">
         <v>0</v>
       </c>
-      <c r="AM39" s="5">
+      <c r="AM39" s="3">
         <v>0</v>
       </c>
       <c r="AN39" s="1">
@@ -5975,8 +6048,8 @@
       <c r="V40" s="1">
         <v>0</v>
       </c>
-      <c r="W40" s="1">
-        <v>0</v>
+      <c r="W40" s="11">
+        <v>1</v>
       </c>
       <c r="X40" s="1">
         <v>0</v>
@@ -6026,7 +6099,7 @@
       <c r="AM40" s="1">
         <v>0</v>
       </c>
-      <c r="AN40" s="5">
+      <c r="AN40" s="3">
         <v>0</v>
       </c>
       <c r="AO40" s="1">
@@ -6160,19 +6233,19 @@
       <c r="AL41" s="1">
         <v>0</v>
       </c>
-      <c r="AM41" s="4">
+      <c r="AM41" s="9">
         <v>1</v>
       </c>
       <c r="AN41" s="1">
         <v>0</v>
       </c>
-      <c r="AO41" s="5">
+      <c r="AO41" s="3">
         <v>0</v>
       </c>
       <c r="AP41" s="1">
         <v>0</v>
       </c>
-      <c r="AQ41" s="4">
+      <c r="AQ41" s="11">
         <v>1</v>
       </c>
       <c r="AR41" s="1">
@@ -6189,10 +6262,10 @@
       <c r="B42" s="1">
         <v>0</v>
       </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
+      <c r="C42" s="6">
+        <v>1</v>
+      </c>
+      <c r="D42" s="6">
         <v>1</v>
       </c>
       <c r="E42" s="1">
@@ -6210,7 +6283,7 @@
       <c r="I42" s="1">
         <v>0</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="11">
         <v>1</v>
       </c>
       <c r="K42" s="1">
@@ -6228,10 +6301,10 @@
       <c r="O42" s="1">
         <v>0</v>
       </c>
-      <c r="P42" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="3">
+      <c r="P42" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="11">
         <v>1</v>
       </c>
       <c r="R42" s="1">
@@ -6306,13 +6379,13 @@
       <c r="AO42" s="1">
         <v>0</v>
       </c>
-      <c r="AP42" s="5">
+      <c r="AP42" s="3">
         <v>0</v>
       </c>
       <c r="AQ42" s="1">
         <v>0</v>
       </c>
-      <c r="AR42" s="3">
+      <c r="AR42" s="6">
         <v>1</v>
       </c>
       <c r="AS42" s="1">
@@ -6371,7 +6444,7 @@
       <c r="Q43" s="1">
         <v>0</v>
       </c>
-      <c r="R43" s="4">
+      <c r="R43" s="9">
         <v>1</v>
       </c>
       <c r="S43" s="1">
@@ -6392,8 +6465,8 @@
       <c r="X43" s="1">
         <v>0</v>
       </c>
-      <c r="Y43" s="1">
-        <v>0</v>
+      <c r="Y43" s="11">
+        <v>1</v>
       </c>
       <c r="Z43" s="1">
         <v>0</v>
@@ -6413,7 +6486,7 @@
       <c r="AE43" s="1">
         <v>0</v>
       </c>
-      <c r="AF43" s="4">
+      <c r="AF43" s="9">
         <v>1</v>
       </c>
       <c r="AG43" s="1">
@@ -6425,7 +6498,7 @@
       <c r="AI43" s="1">
         <v>0</v>
       </c>
-      <c r="AJ43" s="4">
+      <c r="AJ43" s="9">
         <v>1</v>
       </c>
       <c r="AK43" s="1">
@@ -6434,19 +6507,19 @@
       <c r="AL43" s="1">
         <v>0</v>
       </c>
-      <c r="AM43" s="4">
+      <c r="AM43" s="9">
         <v>1</v>
       </c>
       <c r="AN43" s="1">
         <v>0</v>
       </c>
-      <c r="AO43" s="1">
-        <v>0</v>
+      <c r="AO43" s="11">
+        <v>1</v>
       </c>
       <c r="AP43" s="1">
         <v>0</v>
       </c>
-      <c r="AQ43" s="5">
+      <c r="AQ43" s="3">
         <v>0</v>
       </c>
       <c r="AR43" s="1">
@@ -6463,10 +6536,10 @@
       <c r="B44" s="1">
         <v>0</v>
       </c>
-      <c r="C44" s="3">
-        <v>1</v>
-      </c>
-      <c r="D44" s="3">
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6">
         <v>1</v>
       </c>
       <c r="E44" s="1">
@@ -6481,7 +6554,7 @@
       <c r="H44" s="1">
         <v>0</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="10">
         <v>1</v>
       </c>
       <c r="J44" s="1">
@@ -6502,10 +6575,10 @@
       <c r="O44" s="1">
         <v>0</v>
       </c>
-      <c r="P44" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="3">
+      <c r="P44" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="6">
         <v>1</v>
       </c>
       <c r="R44" s="1">
@@ -6526,8 +6599,8 @@
       <c r="W44" s="1">
         <v>0</v>
       </c>
-      <c r="X44" s="1">
-        <v>0</v>
+      <c r="X44" s="11">
+        <v>1</v>
       </c>
       <c r="Y44" s="1">
         <v>0</v>
@@ -6547,19 +6620,19 @@
       <c r="AD44" s="1">
         <v>0</v>
       </c>
-      <c r="AE44" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF44" s="3">
+      <c r="AE44" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF44" s="7">
         <v>1</v>
       </c>
       <c r="AG44" s="1">
         <v>0</v>
       </c>
-      <c r="AH44" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI44" s="3">
+      <c r="AH44" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI44" s="7">
         <v>1</v>
       </c>
       <c r="AJ44" s="1">
@@ -6580,13 +6653,13 @@
       <c r="AO44" s="1">
         <v>0</v>
       </c>
-      <c r="AP44" s="3">
+      <c r="AP44" s="6">
         <v>1</v>
       </c>
       <c r="AQ44" s="1">
         <v>0</v>
       </c>
-      <c r="AR44" s="5">
+      <c r="AR44" s="3">
         <v>0</v>
       </c>
       <c r="AS44" s="1">
@@ -6672,8 +6745,8 @@
       <c r="Z45" s="1">
         <v>0</v>
       </c>
-      <c r="AA45" s="1">
-        <v>0</v>
+      <c r="AA45" s="11">
+        <v>1</v>
       </c>
       <c r="AB45" s="1">
         <v>0</v>
@@ -6726,7 +6799,7 @@
       <c r="AR45" s="1">
         <v>0</v>
       </c>
-      <c r="AS45" s="5">
+      <c r="AS45" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>